<commit_message>
Diagramme avec Références 8209bbdd866f2e0fa4a88a1145daa26e5ab5ed42
</commit_message>
<xml_diff>
--- a/ML/ig/StructureDefinition-ActiviteEnseignement.xlsx
+++ b/ML/ig/StructureDefinition-ActiviteEnseignement.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="103">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-30T15:20:59+00:00</t>
+    <t>2025-10-30T16:36:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -317,6 +317,16 @@
   </si>
   <si>
     <t>Indicateur de suppression de l'autorisation d’activité d’enseignement.</t>
+  </si>
+  <si>
+    <t>ActiviteEnseignement.EntiteGeographique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/mos/StructureDefinition/EntiteGeographique
+</t>
+  </si>
+  <si>
+    <t>Lien vers la classe EntiteGeographique</t>
   </si>
 </sst>
 </file>
@@ -621,7 +631,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -640,7 +650,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="7.6796875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="61.65625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1567,6 +1577,106 @@
         <v>71</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="J10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="K10" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="L10" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="M10" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="S10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="T10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="U10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="V10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="W10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="X10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Y10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="Z10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AF10" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AG10" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH10" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI10" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AJ10" t="s" s="2">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>